<commit_message>
updated sprint 6 backlog
</commit_message>
<xml_diff>
--- a/backlogs/sprint6/backlog.xlsx
+++ b/backlogs/sprint6/backlog.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Unique ID</t>
   </si>
@@ -39,28 +39,28 @@
     <t>As a user, I can view the board members of an application</t>
   </si>
   <si>
-    <t>Omar Khaled</t>
+    <t>Omar El Desouki</t>
   </si>
   <si>
-    <t>Abed Hossam</t>
+    <t>Mostafa Waleed</t>
   </si>
   <si>
-    <t>Ahmed Ashraf</t>
+    <t>Beshoy Raef</t>
   </si>
   <si>
     <t>As an investor or lawyer, I can add or edit board members when creating an application</t>
   </si>
   <si>
-    <t>Mostafa Waleed</t>
+    <t>Omar Khaled</t>
   </si>
   <si>
     <t>As an investor or lawyer, I can edit board members of my application</t>
   </si>
   <si>
-    <t>Yosri Khaled</t>
+    <t>Omar Abdallah</t>
   </si>
   <si>
-    <t>Admin portal</t>
+    <t>Frontend changes</t>
   </si>
   <si>
     <t>As an external entity user, I should be redirected to an admin portal when logging in</t>
@@ -69,31 +69,28 @@
     <t>Ahmed Osama</t>
   </si>
   <si>
-    <t>Translations</t>
+    <t>As a user, I can edit or delete my comments</t>
   </si>
   <si>
-    <t>Implement translation API</t>
+    <t>Yosri Khaled</t>
   </si>
   <si>
-    <t>Omar El Desouki</t>
+    <t>As a user, I can delete my company application</t>
   </si>
   <si>
-    <t>Write translations for all strings</t>
-  </si>
-  <si>
-    <t>Beshoy Raef</t>
-  </si>
-  <si>
-    <t>Implement translation switcher interface</t>
-  </si>
-  <si>
-    <t>Omar Abdallah</t>
+    <t>Abed Hossam</t>
   </si>
   <si>
     <t>Backend</t>
   </si>
   <si>
     <t>Authentication for user controller</t>
+  </si>
+  <si>
+    <t>Ahmed Ashraf</t>
+  </si>
+  <si>
+    <t>Authentication for company controller</t>
   </si>
   <si>
     <t>Authentication for other controllers</t>
@@ -306,119 +303,111 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>2.2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>3.0</v>
+        <v>2.3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2">
-        <v>3.1</v>
-      </c>
-      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>3.2</v>
+        <v>3.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="D12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>4.0</v>
+        <v>3.3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2">
-        <v>4.1</v>
-      </c>
-      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C15" s="2">
         <v>5.0</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>